<commit_message>
Bonus zones for 15/30
</commit_message>
<xml_diff>
--- a/analysis/15_30/data/expanded_sampling_zones.xlsx
+++ b/analysis/15_30/data/expanded_sampling_zones.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
   <si>
     <t>STATIONID</t>
   </si>
@@ -120,6 +120,60 @@
   </si>
   <si>
     <t>Alaska skate</t>
+  </si>
+  <si>
+    <t>TARGET_2</t>
+  </si>
+  <si>
+    <t>U-29</t>
+  </si>
+  <si>
+    <t>U-28</t>
+  </si>
+  <si>
+    <t>U-27</t>
+  </si>
+  <si>
+    <t>U-26</t>
+  </si>
+  <si>
+    <t>J-01</t>
+  </si>
+  <si>
+    <t>I-01</t>
+  </si>
+  <si>
+    <t>H-01</t>
+  </si>
+  <si>
+    <t>G-01</t>
+  </si>
+  <si>
+    <t>H-09</t>
+  </si>
+  <si>
+    <t>H-08</t>
+  </si>
+  <si>
+    <t>H-07</t>
+  </si>
+  <si>
+    <t>H-06</t>
+  </si>
+  <si>
+    <t>Crab</t>
+  </si>
+  <si>
+    <t>M-30</t>
+  </si>
+  <si>
+    <t>M-29</t>
+  </si>
+  <si>
+    <t>M-28</t>
+  </si>
+  <si>
+    <t>M-27</t>
   </si>
 </sst>
 </file>
@@ -439,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +502,7 @@
     <col min="3" max="3" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,167 +512,170 @@
       <c r="C1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
@@ -629,7 +686,7 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -640,7 +697,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
@@ -654,7 +711,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
@@ -668,7 +725,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
@@ -682,7 +739,7 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>21</v>
@@ -696,7 +753,7 @@
         <v>27</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
@@ -707,7 +764,7 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
         <v>26</v>
@@ -718,7 +775,7 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
         <v>26</v>
@@ -729,90 +786,186 @@
         <v>30</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
       <c r="B26">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
       <c r="B27">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
       <c r="B28">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
       <c r="B29">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
       <c r="B30">
         <v>8</v>
       </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
       <c r="B31">
         <v>8</v>
       </c>
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
       <c r="B32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
       <c r="B33">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
       <c r="B34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
       <c r="B35">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
       <c r="B36">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
       <c r="B37">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
       <c r="B38">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
       <c r="B39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
       <c r="B40">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
       <c r="B41">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>